<commit_message>
temp adding sample and record import files
</commit_message>
<xml_diff>
--- a/DPPMasterTemplate.xlsx
+++ b/DPPMasterTemplate.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A15102AB-29DC-419E-935F-D27D274E09B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4C5847-AD6A-4738-A384-131E5B4CF9BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Combined" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,306 +29,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Chakkalakal, Rosette J</author>
-  </authors>
-  <commentList>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{8B684E31-3A17-4B05-8253-484B2D5FB0AF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula here so it updates each week?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{43E8AC35-AC18-40A2-A738-5153C41C127A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula here so it updates each week?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{94AA34E5-26F4-45D3-B14D-3F1EC7D5A833}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula so it updates each week</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{DBAA092B-B4F4-44D5-BDBA-F73F9E81977E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula to calculate</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{A7FE7117-CEF5-4095-A2A0-7A6F17E1FE9D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{1B2FE898-9652-4546-A754-60FCF4FD7B80}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{16D2C2AF-EB90-4BC9-80A4-592DCD265B5E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{531F449F-529F-4DED-95FE-27AE4CB0C399}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-build in formula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{FAE21D79-FA35-4AC9-8BA2-784D7AE33106}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-formula calculates what would be 7% weight loss and what would be 5% weight loss for each group based on total weight of each group (sum all weights of group participants)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{1ABFDA2E-2205-4551-A821-25E0F2170434}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Chakkalakal, Rosette J:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>formula calculates absolute weight loss for the group each week</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{BE20487F-621A-47E9-8395-3253CE005FF1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-General comments:
-- not all info in coach's log is included here--we will likely need to add a few fields (make up session, etc)
-- the master file usually has a separate tab for each coach and then one tab that combines all participants from a given cohort (for example: 3 coaches leading 3 different groups would all be on the combined tab together for people who started in Spring 2019 which is their cohort)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{F6940BE3-ECBC-42A1-BF41-2CA08D7013DA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chakkalakal, Rosette J:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-formula calculates percent weight loss for the group each week</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
@@ -465,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,32 +314,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1470,7 +1144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
   <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1666,6 +1340,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more export functionality
</commit_message>
<xml_diff>
--- a/DPPMasterTemplate.xlsx
+++ b/DPPMasterTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4C5847-AD6A-4738-A384-131E5B4CF9BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF23081-AA9D-42C9-8B5B-17F345C5F14D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>LAST NAME</t>
   </si>
@@ -141,21 +141,6 @@
   </si>
   <si>
     <t>Total sessions attended</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Weekly Wt Loss</t>
-  </si>
-  <si>
-    <t>7% goal</t>
-  </si>
-  <si>
-    <t>Total Wt Loss</t>
-  </si>
-  <si>
-    <t>Percent Loss</t>
   </si>
 </sst>
 </file>
@@ -497,7 +482,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -636,44 +621,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -739,7 +687,7 @@
     <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -762,17 +710,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="58">
@@ -1145,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1121,7 @@
     <col min="36" max="36" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1294,48 +1233,6 @@
       <c r="AK1" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>